<commit_message>
Plantillas para los colores
</commit_message>
<xml_diff>
--- a/docs/color_palette.xlsx
+++ b/docs/color_palette.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="120" yWindow="75" windowWidth="20115" windowHeight="7995"/>
@@ -11,79 +11,81 @@
     <sheet name="Hoja2" sheetId="2" r:id="rId2"/>
     <sheet name="Hoja3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
-  <si>
-    <t>#ffb900</t>
-  </si>
-  <si>
-    <t>#eb790b</t>
-  </si>
-  <si>
-    <t>#ffd240</t>
-  </si>
-  <si>
-    <t>#7464c4</t>
-  </si>
-  <si>
-    <t>#403a96</t>
-  </si>
-  <si>
-    <t>#6536ba</t>
-  </si>
-  <si>
-    <t>#ac009e</t>
-  </si>
-  <si>
-    <t>#00a9ab</t>
-  </si>
-  <si>
-    <t>#0081fb</t>
-  </si>
-  <si>
-    <t>#00c5f8</t>
-  </si>
-  <si>
-    <t>#ff4a65</t>
-  </si>
-  <si>
-    <t>#ef2c35</t>
-  </si>
-  <si>
-    <t>#ff5f60</t>
-  </si>
-  <si>
-    <t>#00be51</t>
-  </si>
-  <si>
-    <t>#009725</t>
-  </si>
-  <si>
-    <t>#00a85b</t>
-  </si>
-  <si>
-    <t>#1e3c4d</t>
-  </si>
-  <si>
-    <t>#00222f</t>
-  </si>
-  <si>
-    <t>#424141</t>
-  </si>
-  <si>
-    <t>#5d5d5d</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+  <si>
+    <t>#ee8435</t>
+  </si>
+  <si>
+    <t>#1957ac</t>
+  </si>
+  <si>
+    <t>#e66016</t>
+  </si>
+  <si>
+    <t>#fdb712</t>
+  </si>
+  <si>
+    <t>#4474e0</t>
+  </si>
+  <si>
+    <t>#0e9860</t>
+  </si>
+  <si>
+    <t>#e588ac</t>
+  </si>
+  <si>
+    <t>#f6a503</t>
+  </si>
+  <si>
+    <t>#00a680</t>
+  </si>
+  <si>
+    <t>#be3737</t>
+  </si>
+  <si>
+    <t>#a8c109</t>
+  </si>
+  <si>
+    <t>#7f928f</t>
+  </si>
+  <si>
+    <t>#9f4180</t>
+  </si>
+  <si>
+    <t>#809a5f</t>
+  </si>
+  <si>
+    <t>#734ff9</t>
+  </si>
+  <si>
+    <t>#35b1c1</t>
+  </si>
+  <si>
+    <t>#d34c41</t>
+  </si>
+  <si>
+    <t>#67298c</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -111,8 +113,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -414,10 +417,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C20"/>
+  <dimension ref="A1:C22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:A20"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -432,11 +435,11 @@
       </c>
       <c r="B1" t="str">
         <f>CONCATENATE("http://netjovenv2.local/assets/css/site/custom/custom_color_", RIGHT(A1,6), ".css")</f>
-        <v>http://netjovenv2.local/assets/css/site/custom/custom_color_ffb900.css</v>
+        <v>http://netjovenv2.local/assets/css/site/custom/custom_color_ee8435.css</v>
       </c>
       <c r="C1" t="str">
         <f>CONCATENATE("insert into njv_color_palette (color, path)  values(","'",A1,"'",",'",B1,"')",";" )</f>
-        <v>insert into njv_color_palette (color, path)  values('#ffb900','http://netjovenv2.local/assets/css/site/custom/custom_color_ffb900.css');</v>
+        <v>insert into njv_color_palette (color, path)  values('#ee8435','http://netjovenv2.local/assets/css/site/custom/custom_color_ee8435.css');</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -444,12 +447,12 @@
         <v>1</v>
       </c>
       <c r="B2" t="str">
-        <f t="shared" ref="B2:B20" si="0">CONCATENATE("http://netjovenv2.local/assets/css/site/custom/custom_color_", RIGHT(A2,6), ".css")</f>
-        <v>http://netjovenv2.local/assets/css/site/custom/custom_color_eb790b.css</v>
+        <f t="shared" ref="B2:B19" si="0">CONCATENATE("http://netjovenv2.local/assets/css/site/custom/custom_color_", RIGHT(A2,6), ".css")</f>
+        <v>http://netjovenv2.local/assets/css/site/custom/custom_color_1957ac.css</v>
       </c>
       <c r="C2" t="str">
-        <f t="shared" ref="C2:C20" si="1">CONCATENATE("insert into njv_color_palette (color, path)  values(","'",A2,"'",",'",B2,"')",";" )</f>
-        <v>insert into njv_color_palette (color, path)  values('#eb790b','http://netjovenv2.local/assets/css/site/custom/custom_color_eb790b.css');</v>
+        <f t="shared" ref="C2:C19" si="1">CONCATENATE("insert into njv_color_palette (color, path)  values(","'",A2,"'",",'",B2,"')",";" )</f>
+        <v>insert into njv_color_palette (color, path)  values('#1957ac','http://netjovenv2.local/assets/css/site/custom/custom_color_1957ac.css');</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -457,12 +460,12 @@
         <v>2</v>
       </c>
       <c r="B3" t="str">
-        <f t="shared" si="0"/>
-        <v>http://netjovenv2.local/assets/css/site/custom/custom_color_ffd240.css</v>
+        <f>CONCATENATE("http://netjovenv2.local/assets/css/site/custom/custom_color_", RIGHT(A3,6), ".css")</f>
+        <v>http://netjovenv2.local/assets/css/site/custom/custom_color_e66016.css</v>
       </c>
       <c r="C3" t="str">
-        <f t="shared" si="1"/>
-        <v>insert into njv_color_palette (color, path)  values('#ffd240','http://netjovenv2.local/assets/css/site/custom/custom_color_ffd240.css');</v>
+        <f>CONCATENATE("insert into njv_color_palette (color, path)  values(","'",A3,"'",",'",B3,"')",";" )</f>
+        <v>insert into njv_color_palette (color, path)  values('#e66016','http://netjovenv2.local/assets/css/site/custom/custom_color_e66016.css');</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -470,12 +473,12 @@
         <v>3</v>
       </c>
       <c r="B4" t="str">
-        <f t="shared" si="0"/>
-        <v>http://netjovenv2.local/assets/css/site/custom/custom_color_7464c4.css</v>
+        <f>CONCATENATE("http://netjovenv2.local/assets/css/site/custom/custom_color_", RIGHT(A4,6), ".css")</f>
+        <v>http://netjovenv2.local/assets/css/site/custom/custom_color_fdb712.css</v>
       </c>
       <c r="C4" t="str">
-        <f t="shared" si="1"/>
-        <v>insert into njv_color_palette (color, path)  values('#7464c4','http://netjovenv2.local/assets/css/site/custom/custom_color_7464c4.css');</v>
+        <f>CONCATENATE("insert into njv_color_palette (color, path)  values(","'",A4,"'",",'",B4,"')",";" )</f>
+        <v>insert into njv_color_palette (color, path)  values('#fdb712','http://netjovenv2.local/assets/css/site/custom/custom_color_fdb712.css');</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -483,12 +486,12 @@
         <v>4</v>
       </c>
       <c r="B5" t="str">
-        <f t="shared" si="0"/>
-        <v>http://netjovenv2.local/assets/css/site/custom/custom_color_403a96.css</v>
+        <f>CONCATENATE("http://netjovenv2.local/assets/css/site/custom/custom_color_", RIGHT(A5,6), ".css")</f>
+        <v>http://netjovenv2.local/assets/css/site/custom/custom_color_4474e0.css</v>
       </c>
       <c r="C5" t="str">
-        <f t="shared" si="1"/>
-        <v>insert into njv_color_palette (color, path)  values('#403a96','http://netjovenv2.local/assets/css/site/custom/custom_color_403a96.css');</v>
+        <f>CONCATENATE("insert into njv_color_palette (color, path)  values(","'",A5,"'",",'",B5,"')",";" )</f>
+        <v>insert into njv_color_palette (color, path)  values('#4474e0','http://netjovenv2.local/assets/css/site/custom/custom_color_4474e0.css');</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -496,12 +499,12 @@
         <v>5</v>
       </c>
       <c r="B6" t="str">
-        <f t="shared" si="0"/>
-        <v>http://netjovenv2.local/assets/css/site/custom/custom_color_6536ba.css</v>
+        <f>CONCATENATE("http://netjovenv2.local/assets/css/site/custom/custom_color_", RIGHT(A6,6), ".css")</f>
+        <v>http://netjovenv2.local/assets/css/site/custom/custom_color_0e9860.css</v>
       </c>
       <c r="C6" t="str">
-        <f t="shared" si="1"/>
-        <v>insert into njv_color_palette (color, path)  values('#6536ba','http://netjovenv2.local/assets/css/site/custom/custom_color_6536ba.css');</v>
+        <f>CONCATENATE("insert into njv_color_palette (color, path)  values(","'",A6,"'",",'",B6,"')",";" )</f>
+        <v>insert into njv_color_palette (color, path)  values('#0e9860','http://netjovenv2.local/assets/css/site/custom/custom_color_0e9860.css');</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -509,12 +512,12 @@
         <v>6</v>
       </c>
       <c r="B7" t="str">
-        <f t="shared" si="0"/>
-        <v>http://netjovenv2.local/assets/css/site/custom/custom_color_ac009e.css</v>
+        <f>CONCATENATE("http://netjovenv2.local/assets/css/site/custom/custom_color_", RIGHT(A7,6), ".css")</f>
+        <v>http://netjovenv2.local/assets/css/site/custom/custom_color_e588ac.css</v>
       </c>
       <c r="C7" t="str">
-        <f t="shared" si="1"/>
-        <v>insert into njv_color_palette (color, path)  values('#ac009e','http://netjovenv2.local/assets/css/site/custom/custom_color_ac009e.css');</v>
+        <f>CONCATENATE("insert into njv_color_palette (color, path)  values(","'",A7,"'",",'",B7,"')",";" )</f>
+        <v>insert into njv_color_palette (color, path)  values('#e588ac','http://netjovenv2.local/assets/css/site/custom/custom_color_e588ac.css');</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -522,12 +525,12 @@
         <v>7</v>
       </c>
       <c r="B8" t="str">
-        <f t="shared" si="0"/>
-        <v>http://netjovenv2.local/assets/css/site/custom/custom_color_00a9ab.css</v>
+        <f>CONCATENATE("http://netjovenv2.local/assets/css/site/custom/custom_color_", RIGHT(A8,6), ".css")</f>
+        <v>http://netjovenv2.local/assets/css/site/custom/custom_color_f6a503.css</v>
       </c>
       <c r="C8" t="str">
-        <f t="shared" si="1"/>
-        <v>insert into njv_color_palette (color, path)  values('#00a9ab','http://netjovenv2.local/assets/css/site/custom/custom_color_00a9ab.css');</v>
+        <f>CONCATENATE("insert into njv_color_palette (color, path)  values(","'",A8,"'",",'",B8,"')",";" )</f>
+        <v>insert into njv_color_palette (color, path)  values('#f6a503','http://netjovenv2.local/assets/css/site/custom/custom_color_f6a503.css');</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -535,12 +538,12 @@
         <v>8</v>
       </c>
       <c r="B9" t="str">
-        <f t="shared" si="0"/>
-        <v>http://netjovenv2.local/assets/css/site/custom/custom_color_0081fb.css</v>
+        <f>CONCATENATE("http://netjovenv2.local/assets/css/site/custom/custom_color_", RIGHT(A9,6), ".css")</f>
+        <v>http://netjovenv2.local/assets/css/site/custom/custom_color_00a680.css</v>
       </c>
       <c r="C9" t="str">
-        <f t="shared" si="1"/>
-        <v>insert into njv_color_palette (color, path)  values('#0081fb','http://netjovenv2.local/assets/css/site/custom/custom_color_0081fb.css');</v>
+        <f>CONCATENATE("insert into njv_color_palette (color, path)  values(","'",A9,"'",",'",B9,"')",";" )</f>
+        <v>insert into njv_color_palette (color, path)  values('#00a680','http://netjovenv2.local/assets/css/site/custom/custom_color_00a680.css');</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -548,12 +551,12 @@
         <v>9</v>
       </c>
       <c r="B10" t="str">
-        <f t="shared" si="0"/>
-        <v>http://netjovenv2.local/assets/css/site/custom/custom_color_00c5f8.css</v>
+        <f>CONCATENATE("http://netjovenv2.local/assets/css/site/custom/custom_color_", RIGHT(A10,6), ".css")</f>
+        <v>http://netjovenv2.local/assets/css/site/custom/custom_color_be3737.css</v>
       </c>
       <c r="C10" t="str">
-        <f t="shared" si="1"/>
-        <v>insert into njv_color_palette (color, path)  values('#00c5f8','http://netjovenv2.local/assets/css/site/custom/custom_color_00c5f8.css');</v>
+        <f>CONCATENATE("insert into njv_color_palette (color, path)  values(","'",A10,"'",",'",B10,"')",";" )</f>
+        <v>insert into njv_color_palette (color, path)  values('#be3737','http://netjovenv2.local/assets/css/site/custom/custom_color_be3737.css');</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
@@ -561,12 +564,12 @@
         <v>10</v>
       </c>
       <c r="B11" t="str">
-        <f t="shared" si="0"/>
-        <v>http://netjovenv2.local/assets/css/site/custom/custom_color_ff4a65.css</v>
+        <f>CONCATENATE("http://netjovenv2.local/assets/css/site/custom/custom_color_", RIGHT(A11,6), ".css")</f>
+        <v>http://netjovenv2.local/assets/css/site/custom/custom_color_a8c109.css</v>
       </c>
       <c r="C11" t="str">
-        <f t="shared" si="1"/>
-        <v>insert into njv_color_palette (color, path)  values('#ff4a65','http://netjovenv2.local/assets/css/site/custom/custom_color_ff4a65.css');</v>
+        <f>CONCATENATE("insert into njv_color_palette (color, path)  values(","'",A11,"'",",'",B11,"')",";" )</f>
+        <v>insert into njv_color_palette (color, path)  values('#a8c109','http://netjovenv2.local/assets/css/site/custom/custom_color_a8c109.css');</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
@@ -574,12 +577,12 @@
         <v>11</v>
       </c>
       <c r="B12" t="str">
-        <f t="shared" si="0"/>
-        <v>http://netjovenv2.local/assets/css/site/custom/custom_color_ef2c35.css</v>
+        <f>CONCATENATE("http://netjovenv2.local/assets/css/site/custom/custom_color_", RIGHT(A12,6), ".css")</f>
+        <v>http://netjovenv2.local/assets/css/site/custom/custom_color_7f928f.css</v>
       </c>
       <c r="C12" t="str">
-        <f t="shared" si="1"/>
-        <v>insert into njv_color_palette (color, path)  values('#ef2c35','http://netjovenv2.local/assets/css/site/custom/custom_color_ef2c35.css');</v>
+        <f>CONCATENATE("insert into njv_color_palette (color, path)  values(","'",A12,"'",",'",B12,"')",";" )</f>
+        <v>insert into njv_color_palette (color, path)  values('#7f928f','http://netjovenv2.local/assets/css/site/custom/custom_color_7f928f.css');</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
@@ -587,12 +590,12 @@
         <v>12</v>
       </c>
       <c r="B13" t="str">
-        <f t="shared" si="0"/>
-        <v>http://netjovenv2.local/assets/css/site/custom/custom_color_ff5f60.css</v>
+        <f>CONCATENATE("http://netjovenv2.local/assets/css/site/custom/custom_color_", RIGHT(A13,6), ".css")</f>
+        <v>http://netjovenv2.local/assets/css/site/custom/custom_color_9f4180.css</v>
       </c>
       <c r="C13" t="str">
-        <f t="shared" si="1"/>
-        <v>insert into njv_color_palette (color, path)  values('#ff5f60','http://netjovenv2.local/assets/css/site/custom/custom_color_ff5f60.css');</v>
+        <f>CONCATENATE("insert into njv_color_palette (color, path)  values(","'",A13,"'",",'",B13,"')",";" )</f>
+        <v>insert into njv_color_palette (color, path)  values('#9f4180','http://netjovenv2.local/assets/css/site/custom/custom_color_9f4180.css');</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
@@ -600,12 +603,12 @@
         <v>13</v>
       </c>
       <c r="B14" t="str">
-        <f t="shared" si="0"/>
-        <v>http://netjovenv2.local/assets/css/site/custom/custom_color_00be51.css</v>
+        <f>CONCATENATE("http://netjovenv2.local/assets/css/site/custom/custom_color_", RIGHT(A14,6), ".css")</f>
+        <v>http://netjovenv2.local/assets/css/site/custom/custom_color_809a5f.css</v>
       </c>
       <c r="C14" t="str">
-        <f t="shared" si="1"/>
-        <v>insert into njv_color_palette (color, path)  values('#00be51','http://netjovenv2.local/assets/css/site/custom/custom_color_00be51.css');</v>
+        <f>CONCATENATE("insert into njv_color_palette (color, path)  values(","'",A14,"'",",'",B14,"')",";" )</f>
+        <v>insert into njv_color_palette (color, path)  values('#809a5f','http://netjovenv2.local/assets/css/site/custom/custom_color_809a5f.css');</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
@@ -613,12 +616,12 @@
         <v>14</v>
       </c>
       <c r="B15" t="str">
-        <f t="shared" si="0"/>
-        <v>http://netjovenv2.local/assets/css/site/custom/custom_color_009725.css</v>
+        <f>CONCATENATE("http://netjovenv2.local/assets/css/site/custom/custom_color_", RIGHT(A15,6), ".css")</f>
+        <v>http://netjovenv2.local/assets/css/site/custom/custom_color_734ff9.css</v>
       </c>
       <c r="C15" t="str">
-        <f t="shared" si="1"/>
-        <v>insert into njv_color_palette (color, path)  values('#009725','http://netjovenv2.local/assets/css/site/custom/custom_color_009725.css');</v>
+        <f>CONCATENATE("insert into njv_color_palette (color, path)  values(","'",A15,"'",",'",B15,"')",";" )</f>
+        <v>insert into njv_color_palette (color, path)  values('#734ff9','http://netjovenv2.local/assets/css/site/custom/custom_color_734ff9.css');</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
@@ -626,12 +629,12 @@
         <v>15</v>
       </c>
       <c r="B16" t="str">
-        <f t="shared" si="0"/>
-        <v>http://netjovenv2.local/assets/css/site/custom/custom_color_00a85b.css</v>
+        <f>CONCATENATE("http://netjovenv2.local/assets/css/site/custom/custom_color_", RIGHT(A16,6), ".css")</f>
+        <v>http://netjovenv2.local/assets/css/site/custom/custom_color_35b1c1.css</v>
       </c>
       <c r="C16" t="str">
-        <f t="shared" si="1"/>
-        <v>insert into njv_color_palette (color, path)  values('#00a85b','http://netjovenv2.local/assets/css/site/custom/custom_color_00a85b.css');</v>
+        <f>CONCATENATE("insert into njv_color_palette (color, path)  values(","'",A16,"'",",'",B16,"')",";" )</f>
+        <v>insert into njv_color_palette (color, path)  values('#35b1c1','http://netjovenv2.local/assets/css/site/custom/custom_color_35b1c1.css');</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
@@ -639,12 +642,12 @@
         <v>16</v>
       </c>
       <c r="B17" t="str">
-        <f t="shared" si="0"/>
-        <v>http://netjovenv2.local/assets/css/site/custom/custom_color_1e3c4d.css</v>
+        <f>CONCATENATE("http://netjovenv2.local/assets/css/site/custom/custom_color_", RIGHT(A17,6), ".css")</f>
+        <v>http://netjovenv2.local/assets/css/site/custom/custom_color_d34c41.css</v>
       </c>
       <c r="C17" t="str">
-        <f t="shared" si="1"/>
-        <v>insert into njv_color_palette (color, path)  values('#1e3c4d','http://netjovenv2.local/assets/css/site/custom/custom_color_1e3c4d.css');</v>
+        <f>CONCATENATE("insert into njv_color_palette (color, path)  values(","'",A17,"'",",'",B17,"')",";" )</f>
+        <v>insert into njv_color_palette (color, path)  values('#d34c41','http://netjovenv2.local/assets/css/site/custom/custom_color_d34c41.css');</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
@@ -652,42 +655,22 @@
         <v>17</v>
       </c>
       <c r="B18" t="str">
-        <f t="shared" si="0"/>
-        <v>http://netjovenv2.local/assets/css/site/custom/custom_color_00222f.css</v>
+        <f>CONCATENATE("http://netjovenv2.local/assets/css/site/custom/custom_color_", RIGHT(A18,6), ".css")</f>
+        <v>http://netjovenv2.local/assets/css/site/custom/custom_color_67298c.css</v>
       </c>
       <c r="C18" t="str">
-        <f t="shared" si="1"/>
-        <v>insert into njv_color_palette (color, path)  values('#00222f','http://netjovenv2.local/assets/css/site/custom/custom_color_00222f.css');</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>18</v>
-      </c>
-      <c r="B19" t="str">
-        <f t="shared" si="0"/>
-        <v>http://netjovenv2.local/assets/css/site/custom/custom_color_424141.css</v>
-      </c>
-      <c r="C19" t="str">
-        <f t="shared" si="1"/>
-        <v>insert into njv_color_palette (color, path)  values('#424141','http://netjovenv2.local/assets/css/site/custom/custom_color_424141.css');</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>19</v>
-      </c>
-      <c r="B20" t="str">
-        <f t="shared" si="0"/>
-        <v>http://netjovenv2.local/assets/css/site/custom/custom_color_5d5d5d.css</v>
-      </c>
-      <c r="C20" t="str">
-        <f t="shared" si="1"/>
-        <v>insert into njv_color_palette (color, path)  values('#5d5d5d','http://netjovenv2.local/assets/css/site/custom/custom_color_5d5d5d.css');</v>
-      </c>
+        <f>CONCATENATE("insert into njv_color_palette (color, path)  values(","'",A18,"'",",'",B18,"')",";" )</f>
+        <v>insert into njv_color_palette (color, path)  values('#67298c','http://netjovenv2.local/assets/css/site/custom/custom_color_67298c.css');</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="20" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B22" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>